<commit_message>
adding header to excel file
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="mySheetName" sheetId="1" r:id="rId1"/>
+    <sheet name="Nodes" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -375,30 +375,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>123</v>
+        <v>Id</v>
       </c>
       <c r="B1" t="str">
-        <v>magic</v>
+        <v>SupplierName</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
+        <v>123</v>
+      </c>
+      <c r="B2" t="str">
+        <v>magic</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
         <v>345</v>
       </c>
-      <c r="B2" t="str">
+      <c r="B3" t="str">
         <v>other</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>